<commit_message>
Confirm Alert and exiting user update password
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19423"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9409898B-3BA8-4AA9-9360-6DC3A7CC8D72}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{48A6A128-A0D4-4661-B97F-743E68C2A80D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,25 +29,25 @@
     <t>email</t>
   </si>
   <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>Moha</t>
-  </si>
-  <si>
-    <t>irfan</t>
-  </si>
-  <si>
-    <t>irfan@gmail.com</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>mohammad</t>
-  </si>
-  <si>
-    <t>mogam@gmil.com</t>
+    <t>newuser</t>
+  </si>
+  <si>
+    <t>Mohammad</t>
+  </si>
+  <si>
+    <t>Irfan</t>
+  </si>
+  <si>
+    <t>irfan22@gmail.com</t>
+  </si>
+  <si>
+    <t>newuser1</t>
+  </si>
+  <si>
+    <t>Farhan</t>
+  </si>
+  <si>
+    <t>farhan@gmil.com</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -451,7 +451,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>

</xml_diff>